<commit_message>
p2p_parser: show bank transfers in the final result in a single column
</commit_message>
<xml_diff>
--- a/tests/expected_results/result_test_write_results_bondora.xlsx
+++ b/tests/expected_results/result_test_write_results_bondora.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tagesergebnisse" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
   <si>
     <t xml:space="preserve">Plattform</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t xml:space="preserve">Endsaldo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ein-/Auszahlungen</t>
   </si>
   <si>
     <t xml:space="preserve">Investitionen</t>
@@ -214,10 +217,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -227,13 +230,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="21.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="11" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="12" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -267,13 +271,16 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="5" t="n">
         <v>43344</v>
@@ -285,21 +292,24 @@
         <v>0.7</v>
       </c>
       <c r="F2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="n">
         <v>-455</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="H2" s="2" t="n">
         <v>282.71</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="I2" s="2" t="n">
         <v>171.8</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="J2" s="2" t="n">
         <v>-12.43</v>
       </c>
-      <c r="J2" s="2" t="n">
+      <c r="K2" s="2" t="n">
         <v>159.37</v>
       </c>
-      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
@@ -314,18 +324,21 @@
         <v>19.6</v>
       </c>
       <c r="F3" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G3" s="2" t="n">
         <v>-1411</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="H3" s="2" t="n">
         <v>265.51</v>
       </c>
-      <c r="H3" s="2" t="n">
+      <c r="I3" s="2" t="n">
         <v>164.38</v>
       </c>
-      <c r="I3" s="2" t="n">
+      <c r="J3" s="2" t="n">
         <v>-18.63</v>
       </c>
-      <c r="J3" s="2" t="n">
+      <c r="K3" s="2" t="n">
         <v>145.75</v>
       </c>
     </row>
@@ -342,18 +355,21 @@
         <v>5.7</v>
       </c>
       <c r="F4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="n">
         <v>-419</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="H4" s="2" t="n">
         <v>238.52</v>
       </c>
-      <c r="H4" s="2" t="n">
+      <c r="I4" s="2" t="n">
         <v>166.58</v>
       </c>
-      <c r="I4" s="2" t="n">
+      <c r="J4" s="2" t="n">
         <v>-44.74</v>
       </c>
-      <c r="J4" s="2" t="n">
+      <c r="K4" s="2" t="n">
         <v>121.84</v>
       </c>
     </row>
@@ -370,18 +386,21 @@
         <v>0.77</v>
       </c>
       <c r="F5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="n">
         <v>-385</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="H5" s="2" t="n">
         <v>188.97</v>
       </c>
-      <c r="H5" s="2" t="n">
+      <c r="I5" s="2" t="n">
         <v>191.1</v>
       </c>
-      <c r="I5" s="2" t="n">
+      <c r="J5" s="2" t="n">
         <v>-41.6</v>
       </c>
-      <c r="J5" s="2" t="n">
+      <c r="K5" s="2" t="n">
         <v>149.51</v>
       </c>
     </row>
@@ -405,10 +424,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -417,13 +436,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="21.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="11" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="12" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -434,7 +454,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
@@ -457,16 +477,19 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>1.19</v>
@@ -475,18 +498,21 @@
         <v>0.7</v>
       </c>
       <c r="F2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="n">
         <v>-455</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="H2" s="2" t="n">
         <v>282.71</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="I2" s="2" t="n">
         <v>171.8</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="J2" s="2" t="n">
         <v>-12.43</v>
       </c>
-      <c r="J2" s="2" t="n">
+      <c r="K2" s="2" t="n">
         <v>159.37</v>
       </c>
     </row>
@@ -494,7 +520,7 @@
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>0.7</v>
@@ -503,18 +529,21 @@
         <v>19.6</v>
       </c>
       <c r="F3" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G3" s="2" t="n">
         <v>-1411</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="H3" s="2" t="n">
         <v>265.51</v>
       </c>
-      <c r="H3" s="2" t="n">
+      <c r="I3" s="2" t="n">
         <v>164.38</v>
       </c>
-      <c r="I3" s="2" t="n">
+      <c r="J3" s="2" t="n">
         <v>-18.63</v>
       </c>
-      <c r="J3" s="2" t="n">
+      <c r="K3" s="2" t="n">
         <v>145.75</v>
       </c>
     </row>
@@ -522,7 +551,7 @@
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>19.6</v>
@@ -531,18 +560,21 @@
         <v>5.7</v>
       </c>
       <c r="F4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="n">
         <v>-419</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="H4" s="2" t="n">
         <v>238.52</v>
       </c>
-      <c r="H4" s="2" t="n">
+      <c r="I4" s="2" t="n">
         <v>166.58</v>
       </c>
-      <c r="I4" s="2" t="n">
+      <c r="J4" s="2" t="n">
         <v>-44.74</v>
       </c>
-      <c r="J4" s="2" t="n">
+      <c r="K4" s="2" t="n">
         <v>121.84</v>
       </c>
     </row>
@@ -550,7 +582,7 @@
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>5.7</v>
@@ -559,18 +591,21 @@
         <v>0.77</v>
       </c>
       <c r="F5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="n">
         <v>-385</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="H5" s="2" t="n">
         <v>188.97</v>
       </c>
-      <c r="H5" s="2" t="n">
+      <c r="I5" s="2" t="n">
         <v>191.1</v>
       </c>
-      <c r="I5" s="2" t="n">
+      <c r="J5" s="2" t="n">
         <v>-41.6</v>
       </c>
-      <c r="J5" s="2" t="n">
+      <c r="K5" s="2" t="n">
         <v>149.51</v>
       </c>
     </row>
@@ -594,10 +629,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -606,13 +641,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="21.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="10" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="11" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -643,13 +679,16 @@
       <c r="I1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>1.19</v>
@@ -658,24 +697,27 @@
         <v>0.77</v>
       </c>
       <c r="E2" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F2" s="2" t="n">
         <v>-2670</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="G2" s="2" t="n">
         <v>975.72</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="H2" s="2" t="n">
         <v>693.87</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="I2" s="2" t="n">
         <v>-117.4</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="J2" s="2" t="n">
         <v>576.47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="2" t="n">
@@ -685,18 +727,21 @@
         <v>0.77</v>
       </c>
       <c r="E3" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F3" s="2" t="n">
         <v>-2670</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="G3" s="2" t="n">
         <v>975.72</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="H3" s="2" t="n">
         <v>693.87</v>
       </c>
-      <c r="H3" s="2" t="n">
+      <c r="I3" s="2" t="n">
         <v>-117.4</v>
       </c>
-      <c r="I3" s="2" t="n">
+      <c r="J3" s="2" t="n">
         <v>576.47</v>
       </c>
     </row>

</xml_diff>